<commit_message>
ReviewDoc ingevuld door Carmen
</commit_message>
<xml_diff>
--- a/src/main/resources/Sprint1/ReviewDoc.xlsx
+++ b/src/main/resources/Sprint1/ReviewDoc.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NN\Documents\vault\src\main\resources\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carme\Documents\Vijf opleidingsonderdelen\Web App\the_Vault\src\main\resources\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FB3E1B-1AFB-4202-9E06-1DE032653B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="12048" yWindow="0" windowWidth="10992" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>MIW-TEAM-2</t>
   </si>
@@ -70,12 +71,30 @@
   </si>
   <si>
     <t>Let op: Code moet voldoen aan de Code Conventions</t>
+  </si>
+  <si>
+    <t>AssetDAO</t>
+  </si>
+  <si>
+    <t>JDBCAssetDAO</t>
+  </si>
+  <si>
+    <t>RootRepository</t>
+  </si>
+  <si>
+    <t>Asset model</t>
+  </si>
+  <si>
+    <t>AssetService</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carmen en </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -418,12 +437,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
+      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -811,36 +830,56 @@
       <c r="E55" s="3"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
+      <c r="A56" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C56" s="2"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
+      <c r="A57" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C57" s="2"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
+      <c r="A58" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C58" s="2"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
+      <c r="A59" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C59" s="2"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
+      <c r="A60" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="C60" s="2"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
@@ -949,7 +988,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$5</xm:f>
           </x14:formula1>
@@ -962,7 +1001,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Klassen klaargezet voor peer review en aanvulling met JavaDoc
</commit_message>
<xml_diff>
--- a/src/main/resources/Sprint1/ReviewDoc.xlsx
+++ b/src/main/resources/Sprint1/ReviewDoc.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carme\Documents\Vijf opleidingsonderdelen\Web App\the_Vault\src\main\resources\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NN\MIW\TheVault\src\main\resources\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E1F138-7739-44AA-BCD9-5B6BA620143A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>MIW-TEAM-2</t>
   </si>
@@ -86,13 +85,28 @@
   </si>
   <si>
     <t>AssetService</t>
+  </si>
+  <si>
+    <t>RekeningDAO</t>
+  </si>
+  <si>
+    <t>JDBCRekeningDAO</t>
+  </si>
+  <si>
+    <t>Model Rekening</t>
+  </si>
+  <si>
+    <t>RekeningService</t>
+  </si>
+  <si>
+    <t>RekeningServiceTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,8 +121,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -118,6 +138,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -149,12 +175,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,25 +462,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="21.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +488,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -468,12 +496,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -490,7 +518,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -501,7 +529,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -512,7 +540,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -521,7 +549,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -532,7 +560,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -543,434 +571,454 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>9</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -983,7 +1031,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$5</xm:f>
           </x14:formula1>
@@ -996,36 +1044,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Klassen klaargezet voor peer review, poging 2
</commit_message>
<xml_diff>
--- a/src/main/resources/Sprint1/ReviewDoc.xlsx
+++ b/src/main/resources/Sprint1/ReviewDoc.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NN\Documents\vault\src\main\resources\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NN\MIW\TheVault\src\main\resources\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>MIW-TEAM-2</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>Support/hashing/BCryptWachwoordHash</t>
+  </si>
+  <si>
+    <t>RekeningDAO</t>
+  </si>
+  <si>
+    <t>JDBCRekeningDAO</t>
+  </si>
+  <si>
+    <t>Model Rekening</t>
+  </si>
+  <si>
+    <t>RekeningService</t>
   </si>
 </sst>
 </file>
@@ -452,20 +464,20 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="37.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,7 +485,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -481,12 +493,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -503,7 +515,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -514,7 +526,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -525,7 +537,7 @@
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -534,7 +546,7 @@
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -545,7 +557,7 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
@@ -556,7 +568,7 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
@@ -567,7 +579,7 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -578,420 +590,436 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="3"/>
       <c r="E52" s="3"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="3"/>
       <c r="E54" s="3"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="3"/>
       <c r="E56" s="3"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="3"/>
       <c r="E57" s="3"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="3"/>
       <c r="E58" s="3"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="3"/>
       <c r="E59" s="3"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="3"/>
       <c r="E60" s="3"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="3"/>
       <c r="E61" s="3"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -1024,29 +1052,29 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
ReviewDoc bewerkt ivm review van Asset klassen en BSN validator en JavaDoc van klassen van Rekening aangepast
</commit_message>
<xml_diff>
--- a/src/main/resources/Sprint1/ReviewDoc.xlsx
+++ b/src/main/resources/Sprint1/ReviewDoc.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>MIW-TEAM-2</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>RekeningService</t>
+  </si>
+  <si>
+    <t>volgens mij wordt de test getest en niet de methode</t>
+  </si>
+  <si>
+    <t>Opmerking</t>
   </si>
 </sst>
 </file>
@@ -145,7 +151,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -168,11 +174,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -180,6 +212,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,45 +497,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -514,72 +564,93 @@
       <c r="E7" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="F7" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="C9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="C11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="9">
+        <v>44538</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -588,10 +659,10 @@
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -599,9 +670,9 @@
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -610,421 +681,422 @@
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>9</v>
+      <c r="A17" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="E18" s="7"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="E20" s="7"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
+      <c r="E22" s="7"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="E23" s="7"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="E24" s="7"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="E26" s="7"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="E27" s="7"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="E30" s="7"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="E31" s="7"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="E32" s="7"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="E33" s="7"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
+      <c r="E34" s="7"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="E35" s="7"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="E36" s="7"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
+      <c r="E37" s="7"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
+      <c r="E38" s="7"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
+      <c r="E39" s="7"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
+      <c r="E40" s="7"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
+      <c r="E41" s="7"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
+      <c r="E42" s="7"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
+      <c r="E43" s="7"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
+      <c r="E44" s="7"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
+      <c r="E45" s="7"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
+      <c r="E46" s="7"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
+      <c r="E47" s="7"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
+      <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
+      <c r="E49" s="7"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
+      <c r="E50" s="7"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
+      <c r="E51" s="7"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
+      <c r="E52" s="7"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
+      <c r="E53" s="7"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
+      <c r="E54" s="7"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
+      <c r="E55" s="7"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
+      <c r="E56" s="7"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
+      <c r="E57" s="7"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
+      <c r="E58" s="7"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
+      <c r="E59" s="7"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
+      <c r="E60" s="7"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
+      <c r="E61" s="7"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
+      <c r="E62" s="7"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
+      <c r="E63" s="7"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
+      <c r="E64" s="7"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
+      <c r="E65" s="7"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
+      <c r="E66" s="7"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
+      <c r="E67" s="7"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
+      <c r="E68" s="7"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
+      <c r="E69" s="7"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
+      <c r="E70" s="7"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
+      <c r="E71" s="7"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
+      <c r="E72" s="7"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
+      <c r="E73" s="7"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
       <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
+      <c r="E74" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
KlantServiceTest opgeschoond en ReviewDoc.xlsx bijgewerkt
</commit_message>
<xml_diff>
--- a/src/main/resources/Sprint1/ReviewDoc.xlsx
+++ b/src/main/resources/Sprint1/ReviewDoc.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carme\Documents\Vijf opleidingsonderdelen\Web App\the_Vault\src\main\resources\Sprint1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8609698E-0204-4A27-9E40-6C1638274C23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
   <si>
     <t>MIW-TEAM-2</t>
   </si>
@@ -112,16 +106,43 @@
     <t>Opmerking</t>
   </si>
   <si>
-    <t>Carmen en</t>
-  </si>
-  <si>
     <t>Document met feedback voor Ju-Sen aangeleverd</t>
+  </si>
+  <si>
+    <t>Carmen en Steven</t>
+  </si>
+  <si>
+    <t>Klantservice</t>
+  </si>
+  <si>
+    <t>KlantDAO</t>
+  </si>
+  <si>
+    <t>JDBCKlantDAO</t>
+  </si>
+  <si>
+    <t>KlantController</t>
+  </si>
+  <si>
+    <t>Steven, Wim en Elise</t>
+  </si>
+  <si>
+    <t>RegistratieService</t>
+  </si>
+  <si>
+    <t>RegistrationDto</t>
+  </si>
+  <si>
+    <t>Model Klant</t>
+  </si>
+  <si>
+    <t>Model Gebruiker</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -227,7 +248,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -497,33 +518,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="47.88671875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="18.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +553,7 @@
       </c>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -541,22 +562,22 @@
       </c>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -576,7 +597,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -590,7 +611,7 @@
       <c r="E8" s="10"/>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -604,18 +625,18 @@
       <c r="E9" s="10"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>18</v>
       </c>
@@ -629,7 +650,7 @@
       <c r="E11" s="10"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
@@ -645,7 +666,7 @@
       <c r="E12" s="10"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
@@ -660,7 +681,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
@@ -671,7 +692,7 @@
       <c r="D14" s="3"/>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" s="12" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
@@ -684,7 +705,7 @@
       <c r="E15" s="10"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" s="12" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>23</v>
       </c>
@@ -698,7 +719,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" s="12" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
@@ -712,7 +733,7 @@
       <c r="E17" s="10"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" s="12" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -727,388 +748,422 @@
       </c>
       <c r="E18" s="10"/>
       <c r="F18" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
       <c r="E19" s="7"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+    <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
       <c r="E20" s="7"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+    <row r="21" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
       <c r="E21" s="7"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+    <row r="22" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="D22" s="3"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+    <row r="23" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="3"/>
       <c r="E23" s="7"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+    <row r="24" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="3"/>
       <c r="E24" s="7"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+    <row r="25" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="3"/>
       <c r="E25" s="7"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+    <row r="26" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C26" s="2"/>
       <c r="D26" s="3"/>
       <c r="E26" s="7"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="3"/>
       <c r="E27" s="7"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
       <c r="E28" s="7"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="3"/>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="3"/>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="3"/>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="3"/>
       <c r="E32" s="7"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="3"/>
       <c r="E33" s="7"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="3"/>
       <c r="E34" s="7"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="3"/>
       <c r="E35" s="7"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="3"/>
       <c r="E36" s="7"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="3"/>
       <c r="E37" s="7"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="3"/>
       <c r="E38" s="7"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="3"/>
       <c r="E39" s="7"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="3"/>
       <c r="E40" s="7"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="3"/>
       <c r="E41" s="7"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="3"/>
       <c r="E42" s="7"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="3"/>
       <c r="E43" s="7"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="3"/>
       <c r="E44" s="7"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="3"/>
       <c r="E45" s="7"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="3"/>
       <c r="E46" s="7"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="3"/>
       <c r="E47" s="7"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="3"/>
       <c r="E48" s="7"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="3"/>
       <c r="E49" s="7"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="3"/>
       <c r="E50" s="7"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="3"/>
       <c r="E51" s="7"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="3"/>
       <c r="E52" s="7"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="3"/>
       <c r="E53" s="7"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="3"/>
       <c r="E54" s="7"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="3"/>
       <c r="E55" s="7"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="3"/>
       <c r="E56" s="7"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="3"/>
       <c r="E57" s="7"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="3"/>
       <c r="E58" s="7"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="3"/>
       <c r="E59" s="7"/>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="3"/>
       <c r="E60" s="7"/>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="3"/>
       <c r="E61" s="7"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
       <c r="D62" s="3"/>
       <c r="E62" s="7"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
       <c r="D63" s="3"/>
       <c r="E63" s="7"/>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="3"/>
       <c r="E64" s="7"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
       <c r="D65" s="3"/>
       <c r="E65" s="7"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
       <c r="D66" s="3"/>
       <c r="E66" s="7"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
       <c r="D67" s="3"/>
       <c r="E67" s="7"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
       <c r="D68" s="3"/>
       <c r="E68" s="7"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
       <c r="D69" s="3"/>
       <c r="E69" s="7"/>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
       <c r="D70" s="3"/>
       <c r="E70" s="7"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
       <c r="D71" s="3"/>
       <c r="E71" s="7"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
       <c r="D72" s="3"/>
       <c r="E72" s="7"/>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -1121,7 +1176,7 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$A$1:$A$5</xm:f>
           </x14:formula1>
@@ -1134,14 +1189,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>